<commit_message>
further fundamentals data clean-up
</commit_message>
<xml_diff>
--- a/SourceData/DataDictionary.xlsx
+++ b/SourceData/DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdc4f9836624c718/Documents/Grad-School-Docs/CapstoneProject/Repo/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_28D3E309B2624BBE1560075AA53AE2C56F2CBADC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DC09617-6242-4D1F-B0FF-13CD7BD07ED5}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_28D3E309B2624BBE1560075AA53AE2C56F2CBADC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D28EC2A-16D3-4C71-9B5A-657AAC050B1A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9276" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fundamentals" sheetId="2" r:id="rId1"/>
@@ -11071,7 +11071,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11081,6 +11081,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11097,12 +11103,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11385,8 +11392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1769"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A901" workbookViewId="0">
-      <selection activeCell="A915" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A743" workbookViewId="0">
+      <selection activeCell="I764" sqref="I764"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15116,82 +15123,82 @@
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A466" t="s">
+      <c r="A466" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="B466" t="s">
+      <c r="B466" s="3" t="s">
         <v>2339</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A467" t="s">
+      <c r="A467" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="B467" t="s">
+      <c r="B467" s="3" t="s">
         <v>2340</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A468" t="s">
+      <c r="A468" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="B468" t="s">
+      <c r="B468" s="3" t="s">
         <v>2341</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A469" t="s">
+      <c r="A469" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="B469" t="s">
+      <c r="B469" s="3" t="s">
         <v>2342</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A470" t="s">
+      <c r="A470" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="B470" t="s">
+      <c r="B470" s="3" t="s">
         <v>2343</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A471" t="s">
+      <c r="A471" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="B471" t="s">
+      <c r="B471" s="3" t="s">
         <v>2344</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A472" t="s">
+      <c r="A472" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="B472" t="s">
+      <c r="B472" s="3" t="s">
         <v>2345</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A473" t="s">
+      <c r="A473" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="B473" t="s">
+      <c r="B473" s="3" t="s">
         <v>2346</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A474" t="s">
+      <c r="A474" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="B474" t="s">
+      <c r="B474" s="3" t="s">
         <v>2347</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A475" t="s">
+      <c r="A475" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="B475" t="s">
+      <c r="B475" s="3" t="s">
         <v>2348</v>
       </c>
     </row>
@@ -15988,106 +15995,106 @@
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A575" t="s">
+      <c r="A575" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="B575" t="s">
+      <c r="B575" s="2" t="s">
         <v>2448</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A576" t="s">
+      <c r="A576" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="B576" t="s">
+      <c r="B576" s="2" t="s">
         <v>2449</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A577" t="s">
+      <c r="A577" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="B577" t="s">
+      <c r="B577" s="2" t="s">
         <v>2450</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A578" t="s">
+      <c r="A578" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="B578" t="s">
+      <c r="B578" s="2" t="s">
         <v>2451</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A579" t="s">
+      <c r="A579" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="B579" t="s">
+      <c r="B579" s="2" t="s">
         <v>2452</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A580" t="s">
+      <c r="A580" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="B580" t="s">
+      <c r="B580" s="2" t="s">
         <v>2453</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A581" t="s">
+      <c r="A581" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="B581" t="s">
+      <c r="B581" s="2" t="s">
         <v>2454</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A582" t="s">
+      <c r="A582" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="B582" t="s">
+      <c r="B582" s="2" t="s">
         <v>2455</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A583" t="s">
+      <c r="A583" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="B583" t="s">
+      <c r="B583" s="2" t="s">
         <v>2456</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A584" t="s">
+      <c r="A584" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="B584" t="s">
+      <c r="B584" s="2" t="s">
         <v>2457</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A585" t="s">
+      <c r="A585" s="2" t="s">
         <v>729</v>
       </c>
-      <c r="B585" t="s">
+      <c r="B585" s="2" t="s">
         <v>2458</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A586" t="s">
+      <c r="A586" s="2" t="s">
         <v>730</v>
       </c>
-      <c r="B586" t="s">
+      <c r="B586" s="2" t="s">
         <v>2459</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A587" t="s">
+      <c r="A587" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="B587" t="s">
+      <c r="B587" s="2" t="s">
         <v>2460</v>
       </c>
     </row>
@@ -17452,50 +17459,50 @@
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A758" t="s">
+      <c r="A758" s="2" t="s">
         <v>902</v>
       </c>
-      <c r="B758" t="s">
+      <c r="B758" s="2" t="s">
         <v>2631</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A759" t="s">
+      <c r="A759" s="2" t="s">
         <v>903</v>
       </c>
-      <c r="B759" t="s">
+      <c r="B759" s="2" t="s">
         <v>2632</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A760" t="s">
+      <c r="A760" s="2" t="s">
         <v>904</v>
       </c>
-      <c r="B760" t="s">
+      <c r="B760" s="2" t="s">
         <v>2633</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A761" t="s">
+      <c r="A761" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="B761" t="s">
+      <c r="B761" s="2" t="s">
         <v>2634</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A762" t="s">
+      <c r="A762" s="2" t="s">
         <v>906</v>
       </c>
-      <c r="B762" t="s">
+      <c r="B762" s="2" t="s">
         <v>2635</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A763" t="s">
+      <c r="A763" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="B763" t="s">
+      <c r="B763" s="2" t="s">
         <v>2636</v>
       </c>
     </row>

</xml_diff>